<commit_message>
added in Soft Duplicate check and KI database
</commit_message>
<xml_diff>
--- a/input/Field team work distribution.xlsx
+++ b/input/Field team work distribution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron.langat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted.sharepoint.com/sites/IMPACTSOM/Documents partages/General/02_Research/01_REACH/Team - Displacement to Durable Solutions (DDS)/03_DDSU/SOMXX_DSA/03_Data_Analysis/DSA_VIII_Scripts/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CE5658-CFF4-41D4-A268-906D01198B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{C9CE5658-CFF4-41D4-A268-906D01198B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51D83A59-C646-405D-A103-E1D9C3454D77}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{9F959C17-EEFE-49A7-9E77-2FDBAFFFADD4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="86">
   <si>
     <t>SN</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Locations</t>
   </si>
   <si>
-    <t>Responsible FO</t>
+    <t>Responsible_FO</t>
   </si>
   <si>
     <t>Southwest</t>
@@ -59,16 +59,13 @@
     <t>Afgooye</t>
   </si>
   <si>
-    <t>Abdikani Kunow/Hassan Abukar</t>
-  </si>
-  <si>
     <t>Jubaland</t>
   </si>
   <si>
     <t>Afmadow</t>
   </si>
   <si>
-    <t>Hajir Abdi</t>
+    <t>Mohamed Kala</t>
   </si>
   <si>
     <t>Baardheere</t>
@@ -83,7 +80,7 @@
     <t>Baki</t>
   </si>
   <si>
-    <t>Abdirahima Barre</t>
+    <t>Mohamed Hassan</t>
   </si>
   <si>
     <t>Hirshabelle</t>
@@ -113,9 +110,6 @@
     <t>Bondhere</t>
   </si>
   <si>
-    <t>Mohamd Kala</t>
-  </si>
-  <si>
     <t>Borama</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Burco</t>
   </si>
   <si>
-    <t>Mohamed Hassan</t>
-  </si>
-  <si>
     <t>Burtinle</t>
   </si>
   <si>
@@ -155,6 +146,9 @@
     <t>Cabudwaaq</t>
   </si>
   <si>
+    <t>Isse Ahad</t>
+  </si>
+  <si>
     <t>Cadaado</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>Ceerigaabo</t>
   </si>
   <si>
-    <t>Dayniile</t>
-  </si>
-  <si>
     <t>Dharkenley</t>
   </si>
   <si>
@@ -191,6 +182,9 @@
     <t>Gaalkacyo</t>
   </si>
   <si>
+    <t>Omar</t>
+  </si>
+  <si>
     <t>Galdogob</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>Karaan</t>
   </si>
   <si>
-    <t>Khada</t>
-  </si>
-  <si>
     <t>Kismaayo</t>
   </si>
   <si>
@@ -290,10 +281,22 @@
     <t>Xudur</t>
   </si>
   <si>
+    <t>Abdikani/Hassan</t>
+  </si>
+  <si>
     <t>Yaaqshid</t>
   </si>
   <si>
     <t>Zeylac</t>
+  </si>
+  <si>
+    <t>Kunow/Hassan</t>
+  </si>
+  <si>
+    <t>Mogadishu Dayniile</t>
+  </si>
+  <si>
+    <t>Mogadishu Khada</t>
   </si>
 </sst>
 </file>
@@ -359,10 +362,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
+<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -400,7 +407,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -506,7 +513,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -648,7 +655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -658,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912084FF-F4EE-4F6A-8FF5-A6783806EA11}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -702,13 +709,13 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -716,13 +723,13 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -733,10 +740,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -744,13 +751,13 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -758,13 +765,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -775,10 +782,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -786,13 +793,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -800,13 +807,13 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -814,24 +821,24 @@
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -839,13 +846,13 @@
         <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -853,13 +860,13 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -867,13 +874,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -881,13 +888,13 @@
         <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -895,13 +902,13 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -909,13 +916,13 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -926,21 +933,21 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -948,13 +955,13 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -962,13 +969,13 @@
         <v>46</v>
       </c>
       <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -976,13 +983,13 @@
         <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -990,13 +997,13 @@
         <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1004,10 +1011,10 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -1015,13 +1022,13 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1029,35 +1036,35 @@
         <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1065,13 +1072,13 @@
         <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1082,10 +1089,10 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1093,13 +1100,13 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1107,13 +1114,13 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1121,13 +1128,13 @@
         <v>41</v>
       </c>
       <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
         <v>26</v>
-      </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1135,13 +1142,13 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1149,35 +1156,35 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
         <v>26</v>
-      </c>
-      <c r="C36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1185,24 +1192,24 @@
         <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1210,24 +1217,24 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1235,13 +1242,13 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1249,35 +1256,35 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D45" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1285,24 +1292,24 @@
         <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
         <v>26</v>
-      </c>
-      <c r="C48" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -1310,13 +1317,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1324,13 +1331,13 @@
         <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1338,13 +1345,13 @@
         <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1355,10 +1362,10 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1366,13 +1373,13 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1383,10 +1390,10 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -1394,24 +1401,24 @@
         <v>36</v>
       </c>
       <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" t="s">
         <v>26</v>
-      </c>
-      <c r="C55" t="s">
-        <v>71</v>
-      </c>
-      <c r="D55" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1419,24 +1426,24 @@
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1444,24 +1451,24 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D59" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D60" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -1472,21 +1479,21 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D62" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1497,21 +1504,21 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -1519,13 +1526,13 @@
         <v>49</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C65" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -1533,24 +1540,24 @@
         <v>49</v>
       </c>
       <c r="B66" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D66" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D67" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -1558,24 +1565,36 @@
         <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D68" xr:uid="{912084FF-F4EE-4F6A-8FF5-A6783806EA11}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064B5BF8B0F90A143B1A4ACAD04008153" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd981dad2fc4ade40153f1adb81431d9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="30973102-2308-455b-8e1f-b6a90edc3b23" xmlns:ns3="947c1918-d5ab-48a1-8b61-0d52f2f99fd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5560d15ed1fa06c5355f4bcdb91e3fc0" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="947c1918-d5ab-48a1-8b61-0d52f2f99fd1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="30973102-2308-455b-8e1f-b6a90edc3b23">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064B5BF8B0F90A143B1A4ACAD04008153" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2d52f37336c5c3d67f6aee7fcfa9c828">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="30973102-2308-455b-8e1f-b6a90edc3b23" xmlns:ns3="947c1918-d5ab-48a1-8b61-0d52f2f99fd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8cb13efdaa903371293ba4bc1418339a" ns2:_="" ns3:_="">
     <xsd:import namespace="30973102-2308-455b-8e1f-b6a90edc3b23"/>
     <xsd:import namespace="947c1918-d5ab-48a1-8b61-0d52f2f99fd1"/>
     <xsd:element name="properties">
@@ -1618,7 +1637,7 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4d06f0b5-5743-41f2-90d3-b12c8ffc7f36" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4d06f0b5-5743-41f2-90d3-b12c8ffc7f36" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -1682,7 +1701,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -1701,7 +1720,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -1718,8 +1737,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1808,7 +1827,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1817,25 +1836,40 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="947c1918-d5ab-48a1-8b61-0d52f2f99fd1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="30973102-2308-455b-8e1f-b6a90edc3b23">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCE887C-AAC8-4870-92E3-3D75A6E045FB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{034456A0-7D7A-4864-850A-49DA0C437707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="947c1918-d5ab-48a1-8b61-0d52f2f99fd1"/>
+    <ds:schemaRef ds:uri="30973102-2308-455b-8e1f-b6a90edc3b23"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D95F33-9790-4A54-82C2-21BD6CB97182}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DBA0D03-8359-4962-9910-F6B15358D856}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="30973102-2308-455b-8e1f-b6a90edc3b23"/>
+    <ds:schemaRef ds:uri="947c1918-d5ab-48a1-8b61-0d52f2f99fd1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{034456A0-7D7A-4864-850A-49DA0C437707}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D95F33-9790-4A54-82C2-21BD6CB97182}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>